<commit_message>
Added a logger to be able to track the rounds. Fixed a few bugs and inconsistencies.
</commit_message>
<xml_diff>
--- a/SimulationNuitDesLegendes/Excel/RepartitionRoles.xlsx
+++ b/SimulationNuitDesLegendes/Excel/RepartitionRoles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\RiderProjects\SimulationNuitDesLegendes\SimulationNuitDesLegendes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C584A5AD-1879-45FD-84E0-96BA166DD153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C8ED6A-9253-492E-8E76-DBB914E36414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11576" xr2:uid="{07565B5C-661B-4722-9AA1-705097393340}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{07565B5C-661B-4722-9AA1-705097393340}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -256,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -288,29 +288,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,22 +646,22 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -673,57 +670,57 @@
       <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="43.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="18" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>5</v>
       </c>
@@ -731,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>12</v>
@@ -739,8 +736,8 @@
       <c r="E3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>12</v>
+      <c r="F3" s="8">
+        <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>12</v>
@@ -751,32 +748,32 @@
       <c r="I3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="18">
-        <f>SUM(B3:I3)</f>
+      <c r="J3" s="13">
+        <f t="shared" ref="J3:J14" si="0">SUM(B3:I3)</f>
         <v>5</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="13">
         <f>SUM(C3,E3,F3,G3,H3,I3)</f>
         <v>4</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="13">
         <f>SUM(B3,D3)</f>
         <v>1</v>
       </c>
-      <c r="M3" s="18" t="str">
-        <f>_xlfn.CONCAT(K3,"/",L3)</f>
+      <c r="M3" s="13" t="str">
+        <f t="shared" ref="M3:M14" si="1">_xlfn.CONCAT(K3,"/",L3)</f>
         <v>4/1</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="13">
         <f>K3/L3</f>
         <v>4</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="13">
         <f>K3-L3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>6</v>
       </c>
@@ -804,32 +801,32 @@
       <c r="I4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="18">
-        <f>SUM(B4:I4)</f>
+      <c r="J4" s="13">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K4" s="18">
-        <f t="shared" ref="K4:K14" si="0">SUM(C4,E4,F4,G4,H4,I4)</f>
+      <c r="K4" s="13">
+        <f t="shared" ref="K4:K14" si="2">SUM(C4,E4,F4,G4,H4,I4)</f>
         <v>5</v>
       </c>
-      <c r="L4" s="18">
-        <f t="shared" ref="L4:L14" si="1">SUM(B4,D4)</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="18" t="str">
-        <f>_xlfn.CONCAT(K4,"/",L4)</f>
+      <c r="L4" s="13">
+        <f t="shared" ref="L4:L14" si="3">SUM(B4,D4)</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="13" t="str">
+        <f t="shared" si="1"/>
         <v>5/1</v>
       </c>
-      <c r="N4" s="18">
-        <f t="shared" ref="N4:N14" si="2">K4/L4</f>
+      <c r="N4" s="13">
+        <f t="shared" ref="N4:N14" si="4">K4/L4</f>
         <v>5</v>
       </c>
-      <c r="O4" s="18">
-        <f t="shared" ref="O4:O14" si="3">K4-L4</f>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:O14" si="5">K4-L4</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>7</v>
       </c>
@@ -857,32 +854,32 @@
       <c r="I5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="18">
-        <f>SUM(B5:I5)</f>
+      <c r="J5" s="13">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K5" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L5" s="18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M5" s="18" t="str">
-        <f>_xlfn.CONCAT(K5,"/",L5)</f>
-        <v>6/1</v>
-      </c>
-      <c r="N5" s="18">
+      <c r="K5" s="13">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="O5" s="18">
+      <c r="L5" s="13">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>6/1</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="O5" s="13">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>8</v>
       </c>
@@ -890,10 +887,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="10">
-        <v>2</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -910,32 +907,32 @@
       <c r="I6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="18">
-        <f>SUM(B6:I6)</f>
+      <c r="J6" s="13">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K6" s="18">
-        <f t="shared" si="0"/>
+      <c r="K6" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="L6" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>7/1</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="L6" s="18">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M6" s="18" t="str">
-        <f>_xlfn.CONCAT(K6,"/",L6)</f>
-        <v>6/2</v>
-      </c>
-      <c r="N6" s="18">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="O6" s="18">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
     </row>
-    <row r="7" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>9</v>
       </c>
@@ -943,10 +940,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -963,32 +960,32 @@
       <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="J7" s="18">
-        <f>SUM(B7:I7)</f>
+      <c r="J7" s="13">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K7" s="18">
-        <f t="shared" si="0"/>
+      <c r="K7" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L7" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>8/1</v>
+      </c>
+      <c r="N7" s="13">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="L7" s="18">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M7" s="18" t="str">
-        <f>_xlfn.CONCAT(K7,"/",L7)</f>
-        <v>7/2</v>
-      </c>
-      <c r="N7" s="18">
-        <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="O7" s="18">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
     </row>
-    <row r="8" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>10</v>
       </c>
@@ -1016,32 +1013,32 @@
       <c r="I8" s="10">
         <v>1</v>
       </c>
-      <c r="J8" s="18">
-        <f>SUM(B8:I8)</f>
+      <c r="J8" s="13">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K8" s="18">
-        <f t="shared" si="0"/>
+      <c r="K8" s="13">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M8" s="18" t="str">
-        <f>_xlfn.CONCAT(K8,"/",L8)</f>
         <v>8/2</v>
       </c>
-      <c r="N8" s="18">
-        <f t="shared" si="2"/>
+      <c r="N8" s="13">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="O8" s="18">
-        <f t="shared" si="3"/>
+      <c r="O8" s="13">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>11</v>
       </c>
@@ -1069,85 +1066,85 @@
       <c r="I9" s="8">
         <v>1</v>
       </c>
-      <c r="J9" s="18">
-        <f>SUM(B9:I9)</f>
+      <c r="J9" s="13">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="L9" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M9" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>9/2</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>12</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L9" s="18">
+        <v>12</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="L10" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M10" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M9" s="18" t="str">
-        <f>_xlfn.CONCAT(K9,"/",L9)</f>
-        <v>9/2</v>
-      </c>
-      <c r="N9" s="18">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="O9" s="18">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>10/2</v>
+      </c>
+      <c r="N10" s="13">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="O10" s="13">
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>12</v>
-      </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10">
-        <v>4</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="18">
-        <f>SUM(B10:I10)</f>
-        <v>12</v>
-      </c>
-      <c r="K10" s="18">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M10" s="18" t="str">
-        <f>_xlfn.CONCAT(K10,"/",L10)</f>
-        <v>9/3</v>
-      </c>
-      <c r="N10" s="18">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="O10" s="18">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>13</v>
       </c>
@@ -1155,52 +1152,52 @@
         <v>1</v>
       </c>
       <c r="C11" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="L11" s="13">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8">
-        <v>1</v>
-      </c>
-      <c r="I11" s="8">
-        <v>1</v>
-      </c>
-      <c r="J11" s="18">
-        <f>SUM(B11:I11)</f>
-        <v>13</v>
-      </c>
-      <c r="K11" s="18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L11" s="18">
+      <c r="M11" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M11" s="18" t="str">
-        <f>_xlfn.CONCAT(K11,"/",L11)</f>
-        <v>10/3</v>
-      </c>
-      <c r="N11" s="18">
-        <f t="shared" si="2"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="O11" s="18">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>11/2</v>
+      </c>
+      <c r="N11" s="13">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="O11" s="13">
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>14</v>
       </c>
@@ -1208,52 +1205,52 @@
         <v>1</v>
       </c>
       <c r="C12" s="10">
+        <v>7</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="L12" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M12" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>12/2</v>
+      </c>
+      <c r="N12" s="13">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="D12" s="10">
-        <v>2</v>
-      </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1</v>
-      </c>
-      <c r="I12" s="10">
-        <v>1</v>
-      </c>
-      <c r="J12" s="18">
-        <f>SUM(B12:I12)</f>
-        <v>14</v>
-      </c>
-      <c r="K12" s="18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L12" s="18">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M12" s="18" t="str">
-        <f>_xlfn.CONCAT(K12,"/",L12)</f>
-        <v>11/3</v>
-      </c>
-      <c r="N12" s="18">
-        <f t="shared" si="2"/>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="O12" s="18">
-        <f t="shared" si="3"/>
-        <v>8</v>
+      <c r="O12" s="13">
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>15</v>
       </c>
@@ -1261,52 +1258,52 @@
         <v>1</v>
       </c>
       <c r="C13" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1</v>
+      </c>
+      <c r="J13" s="13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K13" s="13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="L13" s="13">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="E13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-      <c r="H13" s="8">
-        <v>1</v>
-      </c>
-      <c r="I13" s="8">
-        <v>1</v>
-      </c>
-      <c r="J13" s="18">
-        <f>SUM(B13:I13)</f>
-        <v>15</v>
-      </c>
-      <c r="K13" s="18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L13" s="18">
+      <c r="M13" s="13" t="str">
         <f t="shared" si="1"/>
+        <v>12/3</v>
+      </c>
+      <c r="N13" s="13">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="M13" s="18" t="str">
-        <f>_xlfn.CONCAT(K13,"/",L13)</f>
-        <v>11/4</v>
-      </c>
-      <c r="N13" s="18">
-        <f t="shared" si="2"/>
-        <v>2.75</v>
-      </c>
-      <c r="O13" s="18">
-        <f t="shared" si="3"/>
-        <v>7</v>
+      <c r="O13" s="13">
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16.649999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>16</v>
       </c>
@@ -1314,59 +1311,59 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="L14" s="13">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="E14" s="10">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10">
-        <v>1</v>
-      </c>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
-        <v>1</v>
-      </c>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
-      <c r="J14" s="18">
-        <f>SUM(B14:I14)</f>
-        <v>16</v>
-      </c>
-      <c r="K14" s="18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L14" s="18">
+      <c r="M14" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="M14" s="18" t="str">
-        <f>_xlfn.CONCAT(K14,"/",L14)</f>
-        <v>12/4</v>
-      </c>
-      <c r="N14" s="18">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="O14" s="18">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13/3</v>
+      </c>
+      <c r="N14" s="13">
+        <f t="shared" si="4"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed a few distributions in the Excel file
</commit_message>
<xml_diff>
--- a/SimulationNuitDesLegendes/Excel/RepartitionRoles.xlsx
+++ b/SimulationNuitDesLegendes/Excel/RepartitionRoles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\RiderProjects\SimulationNuitDesLegendes\SimulationNuitDesLegendes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C8ED6A-9253-492E-8E76-DBB914E36414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE9B9DF-674D-47F1-8AC4-0AF3EEFB5B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{07565B5C-661B-4722-9AA1-705097393340}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -646,7 +646,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,10 +940,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="8">
-        <v>3</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
@@ -966,23 +966,23 @@
       </c>
       <c r="K7" s="13">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L7" s="13">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>8/1</v>
+        <v>7/2</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>3.5</v>
       </c>
       <c r="O7" s="13">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>